<commit_message>
add more cases for AutoFill according to org.zkoss.zss.range.impl.autofill.
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/autoFill.xlsx
+++ b/src/main/webapp/WEB-INF/books/autoFill.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27106"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/zssessentials/src/main/webapp/WEB-INF/books/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="17040" windowHeight="11280"/>
+    <workbookView xWindow="45380" yWindow="4220" windowWidth="17040" windowHeight="11280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Auto Fill Sample 1</t>
   </si>
@@ -24,13 +36,46 @@
   </si>
   <si>
     <t>Auto Fill Sample 3</t>
+  </si>
+  <si>
+    <t>Numbers</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Week day</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Month - short</t>
+  </si>
+  <si>
+    <t>Week day - short</t>
+  </si>
+  <si>
+    <t>Janurary</t>
+  </si>
+  <si>
+    <t>Mon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,6 +89,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -87,7 +139,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -98,6 +150,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -106,6 +164,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -152,12 +215,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -184,14 +247,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -218,6 +282,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -393,32 +458,89 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C4:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="19.140625" customWidth="1"/>
+    <col min="3" max="5" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="3:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D5" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E6" s="2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>2007</v>
       </c>
     </row>
   </sheetData>
@@ -426,22 +548,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B2:B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>